<commit_message>
Some night hardcode just to test new lib
</commit_message>
<xml_diff>
--- a/DataGraber.xlsx
+++ b/DataGraber.xlsx
@@ -75,7 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
@@ -88,6 +89,9 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="31.25" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>